<commit_message>
Replace Exit menu option with Quit menuoption, and disabled Enter menu.
</commit_message>
<xml_diff>
--- a/Adventurer/Adv_UseCases/A00_InitExit/A00 GUI Test Summary.xlsx
+++ b/Adventurer/Adv_UseCases/A00_InitExit/A00 GUI Test Summary.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="20" windowWidth="25040" windowHeight="19540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="TA00" sheetId="1" r:id="rId1"/>
@@ -640,10 +640,10 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1037,11 +1037,11 @@
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" ht="72">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18" t="s">
+      <c r="B5" s="19"/>
+      <c r="C5" s="19" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -1053,12 +1053,12 @@
       <c r="F5" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="G5" s="18"/>
+      <c r="G5" s="19"/>
     </row>
     <row r="6" spans="1:7" ht="48">
-      <c r="A6" s="19"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
+      <c r="A6" s="18"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
       <c r="D6" s="4" t="s">
         <v>9</v>
       </c>
@@ -1066,7 +1066,7 @@
       <c r="F6" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="18"/>
+      <c r="G6" s="19"/>
     </row>
     <row r="7" spans="1:7" ht="84">
       <c r="A7" s="5" t="s">
@@ -1195,30 +1195,30 @@
       <c r="G14" s="4"/>
     </row>
     <row r="15" spans="1:7" ht="72">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18" t="s">
+      <c r="B15" s="19"/>
+      <c r="C15" s="19" t="s">
         <v>25</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
     </row>
     <row r="16" spans="1:7" ht="24">
-      <c r="A16" s="19"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
       <c r="D16" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
     </row>
     <row r="17" spans="1:7" ht="36">
       <c r="A17" s="5" t="s">
@@ -1236,14 +1236,14 @@
       <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7" ht="48">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18" t="s">
+      <c r="B18" s="19"/>
+      <c r="C18" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="18" t="s">
+      <c r="D18" s="19" t="s">
         <v>31</v>
       </c>
       <c r="E18" s="20">
@@ -1252,27 +1252,27 @@
       <c r="F18" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G18" s="18"/>
+      <c r="G18" s="19"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="19"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
+      <c r="A19" s="18"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
       <c r="E19" s="20"/>
       <c r="F19" s="4"/>
-      <c r="G19" s="18"/>
+      <c r="G19" s="19"/>
     </row>
     <row r="20" spans="1:7" ht="24">
-      <c r="A20" s="19"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
+      <c r="A20" s="18"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
       <c r="E20" s="20"/>
       <c r="F20" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G20" s="18"/>
+      <c r="G20" s="19"/>
     </row>
     <row r="21" spans="1:7" ht="96">
       <c r="A21" s="5" t="s">
@@ -1780,11 +1780,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="G5:G6"/>
     <mergeCell ref="G15:G16"/>
     <mergeCell ref="A18:A20"/>
     <mergeCell ref="B18:B20"/>
@@ -1797,6 +1792,11 @@
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="E15:E16"/>
     <mergeCell ref="F15:F16"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="G5:G6"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1866,11 +1866,11 @@
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" ht="72">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18" t="s">
+      <c r="B5" s="19"/>
+      <c r="C5" s="19" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="15" t="s">
@@ -1882,12 +1882,12 @@
       <c r="F5" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="G5" s="18"/>
+      <c r="G5" s="19"/>
     </row>
     <row r="6" spans="1:7" ht="48">
-      <c r="A6" s="19"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
+      <c r="A6" s="18"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
       <c r="D6" s="15" t="s">
         <v>9</v>
       </c>
@@ -1895,7 +1895,7 @@
       <c r="F6" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="18"/>
+      <c r="G6" s="19"/>
     </row>
     <row r="7" spans="1:7" ht="84">
       <c r="A7" s="14" t="s">
@@ -2024,30 +2024,30 @@
       <c r="G14" s="15"/>
     </row>
     <row r="15" spans="1:7" ht="72">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18" t="s">
+      <c r="B15" s="19"/>
+      <c r="C15" s="19" t="s">
         <v>25</v>
       </c>
       <c r="D15" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
     </row>
     <row r="16" spans="1:7" ht="24">
-      <c r="A16" s="19"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
       <c r="D16" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
     </row>
     <row r="17" spans="1:7" ht="36">
       <c r="A17" s="14" t="s">
@@ -2065,14 +2065,14 @@
       <c r="G17" s="15"/>
     </row>
     <row r="18" spans="1:7" ht="48">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18" t="s">
+      <c r="B18" s="19"/>
+      <c r="C18" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="18" t="s">
+      <c r="D18" s="19" t="s">
         <v>31</v>
       </c>
       <c r="E18" s="20">
@@ -2081,27 +2081,27 @@
       <c r="F18" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G18" s="18"/>
+      <c r="G18" s="19"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="19"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
+      <c r="A19" s="18"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
       <c r="E19" s="20"/>
       <c r="F19" s="15"/>
-      <c r="G19" s="18"/>
+      <c r="G19" s="19"/>
     </row>
     <row r="20" spans="1:7" ht="24">
-      <c r="A20" s="19"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
+      <c r="A20" s="18"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
       <c r="E20" s="20"/>
       <c r="F20" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="G20" s="18"/>
+      <c r="G20" s="19"/>
     </row>
     <row r="21" spans="1:7" ht="96">
       <c r="A21" s="14" t="s">
@@ -2609,6 +2609,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="G5:G6"/>
     <mergeCell ref="G15:G16"/>
     <mergeCell ref="A18:A20"/>
     <mergeCell ref="B18:B20"/>
@@ -2616,11 +2621,6 @@
     <mergeCell ref="D18:D20"/>
     <mergeCell ref="E18:E20"/>
     <mergeCell ref="G18:G20"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="G5:G6"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="C15:C16"/>

</xml_diff>